<commit_message>
added collabs and improved excel
</commit_message>
<xml_diff>
--- a/F360 Studyplan.xlsx
+++ b/F360 Studyplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Documents\My works\LearnFusion360\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CD4A2F-CCA2-4C78-90AB-5AC23FEBE854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6BAD1C-04B6-4064-97CE-5FD637204AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{917FE661-3C55-431D-91D2-141B86B504FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{917FE661-3C55-431D-91D2-141B86B504FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Day</t>
   </si>
@@ -397,7 +397,7 @@
     <t>Fillet, Chamfer, Shell, Mirror tools, Rectangular, Circular, Mirror patterns</t>
   </si>
   <si>
-    <t>Design a mobile phone stand &amp; a gear wheel with patterned holes</t>
+    <t>Design a gear wheel with patterned holes</t>
   </si>
 </sst>
 </file>
@@ -654,8 +654,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00F46885-7271-4A0F-982D-FE61147C44DC}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0">
-  <autoFilter ref="A1:D36" xr:uid="{00F46885-7271-4A0F-982D-FE61147C44DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00F46885-7271-4A0F-982D-FE61147C44DC}" name="Table1" displayName="Table1" ref="A1:D35" totalsRowShown="0">
+  <autoFilter ref="A1:D35" xr:uid="{00F46885-7271-4A0F-982D-FE61147C44DC}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{418E29E6-125E-4447-8DA2-04C444938EE7}" name="Day" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{607C2101-CA20-408E-818A-C8BC509C167B}" name="Topic" dataDxfId="2"/>
@@ -667,9 +667,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -707,7 +707,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -813,7 +813,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -955,7 +955,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -964,21 +964,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEBB231D-8B42-4045-B4A5-A65E2F22CFD3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.06640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.53125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.53125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.33203125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -992,7 +992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="C2" s="10"/>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1072,10 +1072,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="C9" s="10"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1113,247 +1113,233 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="B24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="B25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="4">
-        <v>10</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="B27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="4">
-        <v>11</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="4">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="B28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
         <v>30</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="4">
-        <v>15</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="4">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="4">
-        <v>17</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="4">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="4">
-        <v>19</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="4">
-        <v>22</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="4">
-        <v>23</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="4">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="4">
-        <v>25</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="4">
-        <v>26</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="B30" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="15" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>